<commit_message>
added cost in dirham
</commit_message>
<xml_diff>
--- a/docs/todo.xlsx
+++ b/docs/todo.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PLDPHEAD\Documents\DEV\spareparts\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dude\Documents\dev\SparepartsMS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA8EFA8-D9BB-42C3-B4FF-8388C99E6049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1963613E-5400-44E8-96FC-8B88663D2DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{32C28D84-F276-44D7-A2C2-BE5CF2903F51}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{32C28D84-F276-44D7-A2C2-BE5CF2903F51}"/>
   </bookViews>
   <sheets>
     <sheet name="todo1" sheetId="1" r:id="rId1"/>
     <sheet name="todo2" sheetId="2" r:id="rId2"/>
-    <sheet name="upgrade" sheetId="3" r:id="rId3"/>
-    <sheet name="clean" sheetId="4" r:id="rId4"/>
+    <sheet name="todo3" sheetId="5" r:id="rId3"/>
+    <sheet name="upgrade" sheetId="3" r:id="rId4"/>
+    <sheet name="clean" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>19. add CODE of part and substitute part number</t>
   </si>
@@ -247,6 +248,33 @@
   </si>
   <si>
     <t>check all project with unit tests and other relevant tests</t>
+  </si>
+  <si>
+    <t>add supplier, Warehouse,Weight Price, USD TO NKF, AED TO USD in the bulk entry reports.</t>
+  </si>
+  <si>
+    <t>description in bulk purchase is not working or having data.</t>
+  </si>
+  <si>
+    <t>reduce stock during addition of loan not during conversion of loan.</t>
+  </si>
+  <si>
+    <t>impliment check status button beside the convert to sale button to check all the payments related to the loan.</t>
+  </si>
+  <si>
+    <t>while converting loans to sale give a choise of payment method. Payment methods could be cash, cheque, transfer. And insert extra info related to the payment method.</t>
+  </si>
+  <si>
+    <t>remove amount and replace with selling price. Total amount = selling price * quantity. Add status to filter.</t>
+  </si>
+  <si>
+    <t>in Point of sale give a choise of payment method. Payment methods could be cash, cheque, transfer. And insert extra info related to the payment method.</t>
+  </si>
+  <si>
+    <t>cheque payment report and transfer payment reports</t>
+  </si>
+  <si>
+    <t>graphs in the dashboard are not displaying correctly. Download all resources, stylesheet and scripts that are refering to cdn servers.</t>
   </si>
 </sst>
 </file>
@@ -319,9 +347,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -359,7 +387,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -465,7 +493,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -607,7 +635,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -621,119 +649,119 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -748,146 +776,146 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566F7387-F463-4289-8172-54255D41BD37}">
   <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="110" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="181.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="181.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -898,6 +926,70 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F45009-85C3-4BD3-9AF6-F5308ABAC757}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="141" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7ED95D-BCB7-4EDB-955D-777FA032910B}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -905,12 +997,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -920,7 +1012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCACF0E3-0CA6-40F3-B6E3-440D1362052E}">
   <dimension ref="A1:A23"/>
   <sheetViews>
@@ -928,99 +1020,99 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>67</v>
       </c>

</xml_diff>